<commit_message>
Correct error in compf
</commit_message>
<xml_diff>
--- a/assets/schedule/frontier.xlsx
+++ b/assets/schedule/frontier.xlsx
@@ -486,7 +486,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Schedule_CF" displayName="Schedule_CF" ref="B3:H22" headerRowCount="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Schedule_CF" displayName="Schedule_CF" ref="B3:H21" headerRowCount="1" totalsRowShown="0">
   <autoFilter ref="B3:H4"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Date" dataDxfId="17"/>
@@ -550,7 +550,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Schedule_CompF" displayName="Schedule_CompF" ref="B3:H16" headerRowCount="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Schedule_CompF" displayName="Schedule_CompF" ref="B3:H17" headerRowCount="1" totalsRowShown="0">
   <autoFilter ref="B3:H4"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Date" dataDxfId="9"/>
@@ -4350,9 +4350,9 @@
       <c r="K166" s="9" t="n"/>
       <c r="L166" s="9" t="n"/>
       <c r="M166" s="9" t="n"/>
-      <c r="N166" s="11" t="inlineStr">
-        <is>
-          <t>CF Industry Session</t>
+      <c r="N166" s="18" t="inlineStr">
+        <is>
+          <t>CompF Industry Session</t>
         </is>
       </c>
       <c r="O166" s="9" t="n"/>
@@ -10780,7 +10780,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:H22"/>
+  <dimension ref="A3:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -11302,62 +11302,62 @@
     <row r="19">
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>7-22</t>
+          <t>7-23</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10:30am-12:30pm</t>
+          <t>8am-12pm</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>JHN 175</t>
+          <t>KNE 130</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>70</v>
+        <v>723</v>
       </c>
       <c r="G19" t="n">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>CF Industry Session</t>
+          <t>CF Report Discussion (23Q)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>7-23</t>
+          <t>7-24</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>8am-12pm</t>
+          <t>8am-10am</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>KNE 130</t>
+          <t>JHN 022</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>723</v>
+        <v>35</v>
       </c>
       <c r="G20" t="n">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>CF Report Discussion (23Q)</t>
+          <t>XF RF-CF RF1 large-volume data analysis and simulation and usage of HPC in data analysis (24B)</t>
         </is>
       </c>
     </row>
@@ -11369,55 +11369,24 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>8am-10am</t>
+          <t>8am-12pm</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>JHN 022</t>
+          <t>KNE 110</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>35</v>
+        <v>223</v>
       </c>
       <c r="G21" t="n">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="H21" t="inlineStr">
-        <is>
-          <t>XF RF-CF RF1 large-volume data analysis and simulation and usage of HPC in data analysis (24B)</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="1" t="inlineStr">
-        <is>
-          <t>7-24</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>8am-12pm</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>4</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>KNE 110</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>223</v>
-      </c>
-      <c r="G22" t="n">
-        <v>200</v>
-      </c>
-      <c r="H22" t="inlineStr">
         <is>
           <t>CF Report Discussion (24M)</t>
         </is>
@@ -13656,7 +13625,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:H16"/>
+  <dimension ref="A3:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -14085,12 +14054,12 @@
     <row r="16">
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>7-23</t>
+          <t>7-22</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>8am-10am</t>
+          <t>10:30am-12:30pm</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -14098,16 +14067,47 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>JHN 075</t>
+          <t>JHN 175</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G16" t="n">
         <v>50</v>
       </c>
       <c r="H16" t="inlineStr">
+        <is>
+          <t>CompF Industry Session</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>7-23</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>8am-10am</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>JHN 075</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>100</v>
+      </c>
+      <c r="G17" t="n">
+        <v>50</v>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>XF TF-CompF QIS (21Z)</t>
         </is>

</xml_diff>

<commit_message>
Add date to the frontier schedule generation
</commit_message>
<xml_diff>
--- a/assets/schedule/frontier.xlsx
+++ b/assets/schedule/frontier.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="600" firstSheet="0" activeTab="12" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Block" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <sheet name="Young" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Key!!" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="current_date">"2022-04-22 23:14:39.737961"</definedName>
+  </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -834,7 +836,7 @@
   </sheetPr>
   <dimension ref="B3:R307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C4"/>
     </sheetView>
   </sheetViews>
@@ -7628,14 +7630,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C4:I32"/>
+  <dimension ref="C2:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
+    <col width="13.9453125" customWidth="1" style="4" min="3" max="3"/>
     <col width="59.41796875" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
     <col width="9.3125" customWidth="1" style="4" min="5" max="5"/>
     <col width="16" customWidth="1" style="4" min="6" max="6"/>
@@ -7643,6 +7646,17 @@
     <col width="10.5234375" bestFit="1" customWidth="1" style="4" min="9" max="9"/>
   </cols>
   <sheetData>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Generated On:</t>
+        </is>
+      </c>
+      <c r="D2">
+        <f>current_date</f>
+        <v/>
+      </c>
+    </row>
     <row r="4">
       <c r="C4" t="inlineStr">
         <is>

</xml_diff>